<commit_message>
Tidied. Added GPS & photodiode code.
</commit_message>
<xml_diff>
--- a/firmware/design/TDMAschema.xlsx
+++ b/firmware/design/TDMAschema.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="39">
   <si>
     <t>DEVICE 1</t>
   </si>
@@ -1832,10 +1832,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1962,48 +1962,48 @@
         <v>30</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -2011,10 +2011,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -2022,10 +2022,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2033,10 +2033,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2044,217 +2044,135 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C19">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="D28" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor changes to packet structure
</commit_message>
<xml_diff>
--- a/firmware/design/TDMAschema.xlsx
+++ b/firmware/design/TDMAschema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial powerup" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="45">
   <si>
     <t>DEVICE 1</t>
   </si>
@@ -120,9 +120,6 @@
     <t>GPS lat</t>
   </si>
   <si>
-    <t>OPTIONAL</t>
-  </si>
-  <si>
     <t>Cloud mean</t>
   </si>
   <si>
@@ -139,6 +136,27 @@
   </si>
   <si>
     <t>PD</t>
+  </si>
+  <si>
+    <t>Status Byte</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>Promiscuous mode</t>
+  </si>
+  <si>
+    <t>GPS valid</t>
+  </si>
+  <si>
+    <t>GPS &gt;3 sat</t>
+  </si>
+  <si>
+    <t>GPS hdop ok</t>
+  </si>
+  <si>
+    <t>SD init ok</t>
   </si>
 </sst>
 </file>
@@ -202,8 +220,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -288,7 +308,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -324,6 +344,7 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -359,6 +380,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1832,15 +1854,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D20" sqref="D20:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="16" max="16" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:16">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1854,8 +1879,35 @@
       <c r="E1" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="3">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3">
+        <v>6</v>
+      </c>
+      <c r="K1" s="3">
+        <v>5</v>
+      </c>
+      <c r="L1" s="3">
+        <v>4</v>
+      </c>
+      <c r="M1" s="3">
+        <v>3</v>
+      </c>
+      <c r="N1" s="3">
+        <v>2</v>
+      </c>
+      <c r="O1" s="3">
+        <v>1</v>
+      </c>
+      <c r="P1" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1865,8 +1917,26 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="H2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1877,18 +1947,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1899,7 +1969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1910,7 +1980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1921,7 +1991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1932,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1943,7 +2013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1954,7 +2024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1965,7 +2035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>14</v>
       </c>
@@ -1976,7 +2046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>15</v>
       </c>
@@ -1987,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>16</v>
       </c>
@@ -1998,7 +2068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>17</v>
       </c>
@@ -2009,7 +2079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:16">
       <c r="A16">
         <v>18</v>
       </c>
@@ -2020,7 +2090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>19</v>
       </c>
@@ -2031,7 +2101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>20</v>
       </c>
@@ -2042,138 +2112,114 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
-      <c r="D22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
-      <c r="D24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
-      <c r="D26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28">
         <v>0</v>
-      </c>
-      <c r="D28" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed GPS transmission. Temperature in one byte.
</commit_message>
<xml_diff>
--- a/firmware/design/TDMAschema.xlsx
+++ b/firmware/design/TDMAschema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial powerup" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="47">
   <si>
     <t>DEVICE 1</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>SD init ok</t>
+  </si>
+  <si>
+    <t>Excess 128 format</t>
+  </si>
+  <si>
+    <t>Ext temp</t>
   </si>
 </sst>
 </file>
@@ -1854,10 +1860,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:D28"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2010,7 +2016,10 @@
         <v>29</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2018,10 +2027,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -2032,147 +2041,147 @@
         <v>30</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2180,45 +2189,23 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27">
-        <v>29</v>
-      </c>
-      <c r="B27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28">
-        <v>30</v>
-      </c>
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revised status criteria & added status byte generation code
</commit_message>
<xml_diff>
--- a/firmware/design/TDMAschema.xlsx
+++ b/firmware/design/TDMAschema.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial powerup" sheetId="1" r:id="rId1"/>
@@ -150,9 +150,6 @@
     <t>GPS valid</t>
   </si>
   <si>
-    <t>GPS &gt;3 sat</t>
-  </si>
-  <si>
     <t>GPS hdop ok</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>Ext temp</t>
+  </si>
+  <si>
+    <t>GPS &gt;=3 sat</t>
   </si>
 </sst>
 </file>
@@ -1863,7 +1863,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1927,13 +1927,13 @@
         <v>39</v>
       </c>
       <c r="L2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="O2" t="s">
         <v>41</v>
@@ -2019,7 +2019,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2203,7 +2203,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26">
         <v>0</v>

</xml_diff>